<commit_message>
add satiation, changes to biol file
</commit_message>
<xml_diff>
--- a/biomass_pools_init_vals.xlsx
+++ b/biomass_pools_init_vals.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11835" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="biomass_pools_init_vals" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="73">
   <si>
     <t>Benthic_grazer_N</t>
   </si>
@@ -219,97 +219,7 @@
     <t>equal distribution with depth &gt; 100m</t>
   </si>
   <si>
-    <t>[1,]</t>
-  </si>
-  <si>
-    <t>[2,]</t>
-  </si>
-  <si>
-    <t>[3,]</t>
-  </si>
-  <si>
-    <t>[4,]</t>
-  </si>
-  <si>
-    <t>[5,]</t>
-  </si>
-  <si>
-    <t>[6,]</t>
-  </si>
-  <si>
-    <t>[7,]</t>
-  </si>
-  <si>
-    <t>[8,]</t>
-  </si>
-  <si>
-    <t>[9,]</t>
-  </si>
-  <si>
-    <t>[10,]</t>
-  </si>
-  <si>
-    <t>[11,]</t>
-  </si>
-  <si>
-    <t>[12,]</t>
-  </si>
-  <si>
-    <t>[13,]</t>
-  </si>
-  <si>
-    <t>[14,]</t>
-  </si>
-  <si>
-    <t>[15,]</t>
-  </si>
-  <si>
-    <t>[16,]</t>
-  </si>
-  <si>
-    <t>[17,]</t>
-  </si>
-  <si>
-    <t>[18,]</t>
-  </si>
-  <si>
-    <t>[19,]</t>
-  </si>
-  <si>
-    <t>[20,]</t>
-  </si>
-  <si>
-    <t>[21,]</t>
-  </si>
-  <si>
-    <t>[22,]</t>
-  </si>
-  <si>
-    <t>[23,]</t>
-  </si>
-  <si>
-    <t>[24,]</t>
-  </si>
-  <si>
-    <t>[25,]</t>
-  </si>
-  <si>
-    <t>[26,]</t>
-  </si>
-  <si>
-    <t>[27,]</t>
-  </si>
-  <si>
-    <t>[28,]</t>
-  </si>
-  <si>
     <t>NaN</t>
-  </si>
-  <si>
-    <t>[29,]</t>
-  </si>
-  <si>
-    <t>[30,]</t>
   </si>
   <si>
     <t>AREA(m2)</t>
@@ -340,7 +250,7 @@
   <numFmts count="1">
     <numFmt numFmtId="168" formatCode="0.000"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -481,14 +391,8 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFC5C8C6"/>
-      <name val="Lucida Console"/>
-      <family val="3"/>
-    </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -674,12 +578,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF1D1F21"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -856,7 +754,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
@@ -864,12 +762,6 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -1201,9 +1093,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S60"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M63" sqref="M63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4847,10 +4741,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF38"/>
+  <dimension ref="A1:AF28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4871,7 +4765,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>63</v>
       </c>
       <c r="B1">
@@ -4883,7 +4777,7 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="I1" s="4" t="s">
-        <v>99</v>
+        <v>69</v>
       </c>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
@@ -4981,193 +4875,193 @@
         <v>8.8999999999999996E-2</v>
       </c>
       <c r="AF2" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
+      <c r="A3" s="8">
         <v>1.083067E-4</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="8">
         <v>3.0580389999999999E-2</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="8">
         <v>-5.1623789999999997E-16</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="8">
         <v>4.14472E-6</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="8">
         <v>4.7219689999999997E-5</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="8">
         <v>2.229151E-3</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="8">
         <v>8.075933E-5</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="8">
         <v>2.514372E-3</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="8">
         <v>5.9465829999999997E-2</v>
       </c>
-      <c r="J3" s="10">
+      <c r="J3" s="8">
         <v>0.13074949999999999</v>
       </c>
-      <c r="K3" s="10">
+      <c r="K3" s="8">
         <v>0.30248510000000001</v>
       </c>
-      <c r="L3" s="10">
+      <c r="L3" s="8">
         <v>5.3018290000000001E-4</v>
       </c>
-      <c r="M3" s="10">
+      <c r="M3" s="8">
         <v>0.31595200000000001</v>
       </c>
-      <c r="N3" s="10">
+      <c r="N3" s="8">
         <v>5.8977300000000003E-4</v>
       </c>
-      <c r="O3" s="10">
+      <c r="O3" s="8">
         <v>8.5590240000000001E-3</v>
       </c>
-      <c r="P3" s="10">
+      <c r="P3" s="8">
         <v>2.4154990000000001E-2</v>
       </c>
-      <c r="Q3" s="10">
+      <c r="Q3" s="8">
         <v>1.0789860000000001E-3</v>
       </c>
-      <c r="R3" s="10">
+      <c r="R3" s="8">
         <v>1.8113730000000001E-2</v>
       </c>
-      <c r="S3" s="10">
+      <c r="S3" s="8">
         <v>1.2349550000000001E-2</v>
       </c>
-      <c r="T3" s="10">
+      <c r="T3" s="8">
         <v>2.6331760000000001E-3</v>
       </c>
-      <c r="U3" s="10">
+      <c r="U3" s="8">
         <v>2.6721660000000001E-4</v>
       </c>
-      <c r="V3" s="10">
+      <c r="V3" s="8">
         <v>4.3963509999999997E-3</v>
       </c>
-      <c r="W3" s="10">
+      <c r="W3" s="8">
         <v>2.7584290000000001E-2</v>
       </c>
-      <c r="X3" s="10">
+      <c r="X3" s="8">
         <v>7.4017670000000001E-3</v>
       </c>
-      <c r="Y3" s="10">
+      <c r="Y3" s="8">
         <v>1.2460710000000001E-3</v>
       </c>
-      <c r="Z3" s="10">
+      <c r="Z3" s="8">
         <v>6.2941469999999999E-3</v>
       </c>
-      <c r="AA3" s="10">
+      <c r="AA3" s="8">
         <v>3.074902E-3</v>
       </c>
-      <c r="AB3" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="AC3" s="10">
+      <c r="AB3" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC3" s="8">
         <v>2.1983469999999998E-3</v>
       </c>
-      <c r="AD3" s="10">
+      <c r="AD3" s="8">
         <v>3.6187070000000002E-2</v>
       </c>
       <c r="AF3" t="s">
-        <v>101</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A4" s="11">
-        <v>0</v>
-      </c>
-      <c r="B4" s="11">
-        <v>1</v>
-      </c>
-      <c r="C4" s="11">
+      <c r="A4" s="9">
+        <v>0</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9">
         <v>2</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="9">
         <v>3</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="9">
         <v>4</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="9">
         <v>5</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="9">
         <v>6</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="9">
         <v>7</v>
       </c>
-      <c r="I4" s="11">
+      <c r="I4" s="9">
         <v>8</v>
       </c>
-      <c r="J4" s="11">
+      <c r="J4" s="9">
         <v>9</v>
       </c>
-      <c r="K4" s="11">
+      <c r="K4" s="9">
         <v>10</v>
       </c>
-      <c r="L4" s="11">
+      <c r="L4" s="9">
         <v>11</v>
       </c>
-      <c r="M4" s="11">
+      <c r="M4" s="9">
         <v>12</v>
       </c>
-      <c r="N4" s="11">
+      <c r="N4" s="9">
         <v>13</v>
       </c>
-      <c r="O4" s="11">
+      <c r="O4" s="9">
         <v>14</v>
       </c>
-      <c r="P4" s="11">
+      <c r="P4" s="9">
         <v>15</v>
       </c>
-      <c r="Q4" s="11">
+      <c r="Q4" s="9">
         <v>16</v>
       </c>
-      <c r="R4" s="11">
+      <c r="R4" s="9">
         <v>17</v>
       </c>
-      <c r="S4" s="11">
+      <c r="S4" s="9">
         <v>18</v>
       </c>
-      <c r="T4" s="11">
+      <c r="T4" s="9">
         <v>19</v>
       </c>
-      <c r="U4" s="11">
+      <c r="U4" s="9">
         <v>20</v>
       </c>
-      <c r="V4" s="11">
+      <c r="V4" s="9">
         <v>21</v>
       </c>
-      <c r="W4" s="11">
+      <c r="W4" s="9">
         <v>22</v>
       </c>
-      <c r="X4" s="11">
+      <c r="X4" s="9">
         <v>23</v>
       </c>
-      <c r="Y4" s="11">
+      <c r="Y4" s="9">
         <v>24</v>
       </c>
-      <c r="Z4" s="11">
+      <c r="Z4" s="9">
         <v>25</v>
       </c>
-      <c r="AA4" s="11">
+      <c r="AA4" s="9">
         <v>26</v>
       </c>
-      <c r="AB4" s="11">
+      <c r="AB4" s="9">
         <v>27</v>
       </c>
-      <c r="AC4" s="11">
+      <c r="AC4" s="9">
         <v>28</v>
       </c>
-      <c r="AD4" s="11">
+      <c r="AD4" s="9">
         <v>29</v>
       </c>
       <c r="AF4" t="s">
@@ -5175,594 +5069,460 @@
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+      <c r="A5" s="7">
         <v>12647072876.070601</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="7">
         <v>12286957937.1882</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="7">
         <v>29971254485.736198</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="7">
         <v>13938887159.594101</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="7">
         <v>3686010853.0107198</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="7">
         <v>11079367894.924</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="7">
         <v>19434502995.363899</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="7">
         <v>10361542520.3428</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="7">
         <v>6455559422.1001797</v>
       </c>
-      <c r="J5" s="9">
+      <c r="J5" s="7">
         <v>17316802510.668701</v>
       </c>
-      <c r="K5" s="9">
+      <c r="K5" s="7">
         <v>11225017827.105801</v>
       </c>
-      <c r="L5" s="9">
+      <c r="L5" s="7">
         <v>15989283040.5315</v>
       </c>
-      <c r="M5" s="9">
+      <c r="M5" s="7">
         <v>4282287422.5834799</v>
       </c>
-      <c r="N5" s="9">
+      <c r="N5" s="7">
         <v>14161620804.7365</v>
       </c>
-      <c r="O5" s="9">
+      <c r="O5" s="7">
         <v>12608709589.035801</v>
       </c>
-      <c r="P5" s="9">
+      <c r="P5" s="7">
         <v>9175347754.5618896</v>
       </c>
-      <c r="Q5" s="9">
+      <c r="Q5" s="7">
         <v>11324453300.625099</v>
       </c>
-      <c r="R5" s="9">
+      <c r="R5" s="7">
         <v>5030841127.8167295</v>
       </c>
-      <c r="S5" s="9">
+      <c r="S5" s="7">
         <v>4831356901.1825304</v>
       </c>
-      <c r="T5" s="9">
+      <c r="T5" s="7">
         <v>17683470543.246601</v>
       </c>
-      <c r="U5" s="9">
+      <c r="U5" s="7">
         <v>9957085305.7049599</v>
       </c>
-      <c r="V5" s="9">
+      <c r="V5" s="7">
         <v>6033778735.8615398</v>
       </c>
-      <c r="W5" s="9">
+      <c r="W5" s="7">
         <v>17242902544.7892</v>
       </c>
-      <c r="X5" s="9">
+      <c r="X5" s="7">
         <v>173026052.579703</v>
       </c>
-      <c r="Y5" s="9">
+      <c r="Y5" s="7">
         <v>294595431.74642199</v>
       </c>
-      <c r="Z5" s="9">
+      <c r="Z5" s="7">
         <v>35556339823.5214</v>
       </c>
-      <c r="AA5" s="9">
+      <c r="AA5" s="7">
         <v>17529276725.053299</v>
       </c>
-      <c r="AB5" s="9">
+      <c r="AB5" s="7">
         <v>26033456847.904099</v>
       </c>
-      <c r="AC5" s="9">
+      <c r="AC5" s="7">
         <v>40232596618.555801</v>
       </c>
-      <c r="AD5" s="9">
+      <c r="AD5" s="7">
         <v>27427742420.496799</v>
       </c>
       <c r="AF5" t="s">
-        <v>96</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <f>A3*63000*1000000000/20/5.7</f>
-        <v>59853702.631578937</v>
+        <f>A9*63000*1000000000/20/5.7</f>
+        <v>-2.6891356578947361E-4</v>
       </c>
       <c r="B6" s="1">
-        <f t="shared" ref="B6:AD6" si="0">B3*63000*1000000000/20/5.7</f>
-        <v>16899689210.526316</v>
+        <f t="shared" ref="B6:AD6" si="0">B9*63000*1000000000/20/5.7</f>
+        <v>-2.7390371842105261E-4</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" si="0"/>
-        <v>-2.8528936578947367E-4</v>
+        <v>700137789.47368419</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="0"/>
-        <v>2290503.1578947371</v>
+        <v>13115146578.947369</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>26095091.842105258</v>
+        <v>263393660.52631581</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="0"/>
-        <v>1231899236.8421052</v>
+        <v>9618707.3684210517</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" si="0"/>
-        <v>44630156.052631579</v>
+        <v>169814013.1578947</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="0"/>
-        <v>1389521368.4210527</v>
+        <v>255598073.68421051</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="0"/>
-        <v>32862695526.315784</v>
+        <v>18237212368.421051</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="0"/>
-        <v>72256302631.578934</v>
+        <v>1032471631.5789472</v>
       </c>
       <c r="K6" s="1">
         <f t="shared" si="0"/>
-        <v>167162818421.05261</v>
+        <v>657295578.94736838</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" si="0"/>
-        <v>292995813.15789473</v>
+        <v>10488919736.842106</v>
       </c>
       <c r="M6" s="1">
         <f t="shared" si="0"/>
-        <v>174605052631.57898</v>
+        <v>-1.7188289999999997E-4</v>
       </c>
       <c r="N6" s="1">
         <f t="shared" si="0"/>
-        <v>325927184.21052641</v>
+        <v>4617816552.6315794</v>
       </c>
       <c r="O6" s="1">
         <f t="shared" si="0"/>
-        <v>4729986947.3684216</v>
+        <v>767143815.78947365</v>
       </c>
       <c r="P6" s="1">
         <f t="shared" si="0"/>
-        <v>13348810263.157894</v>
+        <v>3458483368.4210525</v>
       </c>
       <c r="Q6" s="1">
         <f t="shared" si="0"/>
-        <v>596281736.84210527</v>
-      </c>
-      <c r="R6" s="1">
+        <v>582831789.47368419</v>
+      </c>
+      <c r="R6" s="1" t="e">
         <f t="shared" si="0"/>
-        <v>10010219210.526316</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S6" s="1">
         <f t="shared" si="0"/>
-        <v>6824751315.7894735</v>
+        <v>8522739473.6842089</v>
       </c>
       <c r="T6" s="1">
         <f t="shared" si="0"/>
-        <v>1455176210.5263162</v>
+        <v>19801607368.421051</v>
       </c>
       <c r="U6" s="1">
         <f t="shared" si="0"/>
-        <v>147672331.57894737</v>
+        <v>58394589473.684212</v>
       </c>
       <c r="V6" s="1">
         <f t="shared" si="0"/>
-        <v>2429562394.7368412</v>
+        <v>189966884210.52631</v>
       </c>
       <c r="W6" s="1">
         <f t="shared" si="0"/>
-        <v>15243949736.842104</v>
+        <v>220642413157.89474</v>
       </c>
       <c r="X6" s="1">
         <f t="shared" si="0"/>
-        <v>4090450184.210526</v>
+        <v>221417202.63157898</v>
       </c>
       <c r="Y6" s="1">
         <f t="shared" si="0"/>
-        <v>688618184.21052647</v>
+        <v>-2.9026028684210527E-4</v>
       </c>
       <c r="Z6" s="1">
         <f t="shared" si="0"/>
-        <v>3478344394.7368422</v>
+        <v>6.5426384210526316E-5</v>
       </c>
       <c r="AA6" s="1">
         <f t="shared" si="0"/>
-        <v>1699287947.3684211</v>
-      </c>
-      <c r="AB6" s="1" t="e">
+        <v>190161576.31578946</v>
+      </c>
+      <c r="AB6" s="1">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>-2.5255694210526313E-4</v>
       </c>
       <c r="AC6" s="1">
         <f t="shared" si="0"/>
-        <v>1214875973.6842105</v>
+        <v>63318536.842105262</v>
       </c>
       <c r="AD6" s="1">
         <f t="shared" si="0"/>
-        <v>19998117631.578945</v>
+        <v>11212574.210526315</v>
       </c>
       <c r="AF6" t="s">
-        <v>98</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A7" s="12">
+      <c r="A7" s="10">
         <f>A6/A5</f>
-        <v>4.7326130890593286E-3</v>
-      </c>
-      <c r="B7" s="12">
+        <v>-2.1262909483053765E-14</v>
+      </c>
+      <c r="B7" s="10">
         <f t="shared" ref="B7:AD7" si="1">B6/B5</f>
-        <v>1.3754168685950359</v>
-      </c>
-      <c r="C7" s="12">
+        <v>-2.2292232122976887E-14</v>
+      </c>
+      <c r="C7" s="10">
         <f t="shared" si="1"/>
-        <v>-9.5187662540200807E-15</v>
-      </c>
-      <c r="D7" s="12">
+        <v>2.3360309786395195E-2</v>
+      </c>
+      <c r="D7" s="10">
         <f t="shared" si="1"/>
-        <v>1.6432467898401699E-4</v>
-      </c>
-      <c r="E7" s="12">
+        <v>0.94090341852866255</v>
+      </c>
+      <c r="E7" s="10">
         <f t="shared" si="1"/>
-        <v>7.0794940337169342E-3</v>
-      </c>
-      <c r="F7" s="12">
+        <v>7.1457646499108074E-2</v>
+      </c>
+      <c r="F7" s="10">
         <f t="shared" si="1"/>
-        <v>0.11118858481145828</v>
-      </c>
-      <c r="G7" s="12">
+        <v>8.6816391148342067E-4</v>
+      </c>
+      <c r="G7" s="10">
         <f t="shared" si="1"/>
-        <v>2.296439279320809E-3</v>
-      </c>
-      <c r="H7" s="12">
+        <v>8.7377594990931257E-3</v>
+      </c>
+      <c r="H7" s="10">
         <f t="shared" si="1"/>
-        <v>0.1341037172499179</v>
-      </c>
-      <c r="I7" s="12">
+        <v>2.4667955874561651E-2</v>
+      </c>
+      <c r="I7" s="10">
         <f t="shared" si="1"/>
-        <v>5.0906038311432047</v>
-      </c>
-      <c r="J7" s="12">
+        <v>2.8250398108004648</v>
+      </c>
+      <c r="J7" s="10">
         <f t="shared" si="1"/>
-        <v>4.1726122699073676</v>
-      </c>
-      <c r="K7" s="12">
+        <v>5.9622533140448547E-2</v>
+      </c>
+      <c r="K7" s="10">
         <f t="shared" si="1"/>
-        <v>14.891986898888783</v>
-      </c>
-      <c r="L7" s="12">
+        <v>5.8556306018521666E-2</v>
+      </c>
+      <c r="L7" s="10">
         <f t="shared" si="1"/>
-        <v>1.8324512263318798E-2</v>
-      </c>
-      <c r="M7" s="12">
+        <v>0.65599687679888885</v>
+      </c>
+      <c r="M7" s="10">
         <f t="shared" si="1"/>
-        <v>40.773781720200539</v>
-      </c>
-      <c r="N7" s="12">
+        <v>-4.0138104484426223E-14</v>
+      </c>
+      <c r="N7" s="10">
         <f t="shared" si="1"/>
-        <v>2.3014822152385036E-2</v>
-      </c>
-      <c r="O7" s="12">
+        <v>0.32607966392428067</v>
+      </c>
+      <c r="O7" s="10">
         <f t="shared" si="1"/>
-        <v>0.3751364811734178</v>
-      </c>
-      <c r="P7" s="12">
+        <v>6.0842373311267441E-2</v>
+      </c>
+      <c r="P7" s="10">
         <f t="shared" si="1"/>
-        <v>1.454856057801297</v>
-      </c>
-      <c r="Q7" s="12">
+        <v>0.37693212954261374</v>
+      </c>
+      <c r="Q7" s="10">
         <f t="shared" si="1"/>
-        <v>5.2654350811724489E-2</v>
-      </c>
-      <c r="R7" s="12">
-        <f t="shared" si="1"/>
-        <v>1.9897704889103749</v>
-      </c>
-      <c r="S7" s="12">
-        <f t="shared" si="1"/>
-        <v>1.4125951477770224</v>
-      </c>
-      <c r="T7" s="12">
-        <f t="shared" si="1"/>
-        <v>8.2290193373950271E-2</v>
-      </c>
-      <c r="U7" s="12">
-        <f t="shared" si="1"/>
-        <v>1.4830879423553578E-2</v>
-      </c>
-      <c r="V7" s="12">
-        <f t="shared" si="1"/>
-        <v>0.40266017384708314</v>
-      </c>
-      <c r="W7" s="12">
-        <f t="shared" si="1"/>
-        <v>0.88407097918956934</v>
-      </c>
-      <c r="X7" s="12">
-        <f t="shared" si="1"/>
-        <v>23.640660601248442</v>
-      </c>
-      <c r="Y7" s="12">
-        <f t="shared" si="1"/>
-        <v>2.3375046249979405</v>
-      </c>
-      <c r="Z7" s="12">
-        <f t="shared" si="1"/>
-        <v>9.7826278295265676E-2</v>
-      </c>
-      <c r="AA7" s="12">
-        <f t="shared" si="1"/>
-        <v>9.6939992107019132E-2</v>
-      </c>
-      <c r="AB7" s="12" t="e">
+        <v>5.1466660155816302E-2</v>
+      </c>
+      <c r="R7" s="10" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AC7" s="12">
+      <c r="S7" s="10">
         <f t="shared" si="1"/>
-        <v>3.0196310350097906E-2</v>
-      </c>
-      <c r="AD7" s="12">
+        <v>1.7640467570504199</v>
+      </c>
+      <c r="T7" s="10">
         <f t="shared" si="1"/>
-        <v>0.72912007576074933</v>
+        <v>1.119780606414015</v>
+      </c>
+      <c r="U7" s="10">
+        <f t="shared" si="1"/>
+        <v>5.8646268140563933</v>
+      </c>
+      <c r="V7" s="10">
+        <f t="shared" si="1"/>
+        <v>31.483899646744614</v>
+      </c>
+      <c r="W7" s="10">
+        <f t="shared" si="1"/>
+        <v>12.796129455859671</v>
+      </c>
+      <c r="X7" s="10">
+        <f t="shared" si="1"/>
+        <v>1.2796755131981352</v>
+      </c>
+      <c r="Y7" s="10">
+        <f t="shared" si="1"/>
+        <v>-9.8528441232568657E-13</v>
+      </c>
+      <c r="Z7" s="10">
+        <f t="shared" si="1"/>
+        <v>1.8400764683671163E-15</v>
+      </c>
+      <c r="AA7" s="10">
+        <f t="shared" si="1"/>
+        <v>1.0848227185780322E-2</v>
+      </c>
+      <c r="AB7" s="10">
+        <f t="shared" si="1"/>
+        <v>-9.7012449626180169E-15</v>
+      </c>
+      <c r="AC7" s="10">
+        <f t="shared" si="1"/>
+        <v>1.5738118382570892E-3</v>
+      </c>
+      <c r="AD7" s="10">
+        <f t="shared" si="1"/>
+        <v>4.0880412389125909E-4</v>
       </c>
       <c r="AF7" t="s">
-        <v>97</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>65</v>
+      <c r="A9" s="1">
+        <v>-4.8660549999999996E-16</v>
       </c>
       <c r="B9" s="1">
-        <v>1.083067E-4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>66</v>
-      </c>
-      <c r="B10" s="1">
-        <v>3.0580389999999999E-2</v>
+        <v>-4.9563529999999996E-16</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1.2669160000000001E-3</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2.373217E-2</v>
+      </c>
+      <c r="E9" s="1">
+        <v>4.7661710000000001E-4</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1.7405279999999999E-5</v>
+      </c>
+      <c r="G9" s="1">
+        <v>3.0728249999999998E-4</v>
+      </c>
+      <c r="H9" s="1">
+        <v>4.6251080000000002E-4</v>
+      </c>
+      <c r="I9" s="1">
+        <v>3.3000670000000003E-2</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1.868282E-3</v>
+      </c>
+      <c r="K9" s="1">
+        <v>1.1893920000000001E-3</v>
+      </c>
+      <c r="L9" s="1">
+        <v>1.8979949999999999E-2</v>
+      </c>
+      <c r="M9" s="1">
+        <v>-3.1102619999999999E-16</v>
+      </c>
+      <c r="N9" s="1">
+        <v>8.3560490000000008E-3</v>
+      </c>
+      <c r="O9" s="1">
+        <v>1.388165E-3</v>
+      </c>
+      <c r="P9" s="1">
+        <v>6.2582080000000003E-3</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>1.054648E-3</v>
+      </c>
+      <c r="R9" t="s">
+        <v>17</v>
+      </c>
+      <c r="S9" s="1">
+        <v>1.5422099999999999E-2</v>
+      </c>
+      <c r="T9" s="1">
+        <v>3.5831479999999999E-2</v>
+      </c>
+      <c r="U9" s="1">
+        <v>0.10566639999999999</v>
+      </c>
+      <c r="V9" s="1">
+        <v>0.34374959999999999</v>
+      </c>
+      <c r="W9" s="1">
+        <v>0.39925769999999999</v>
+      </c>
+      <c r="X9" s="1">
+        <v>4.0065970000000001E-4</v>
+      </c>
+      <c r="Y9" s="1">
+        <v>-5.2523290000000003E-16</v>
+      </c>
+      <c r="Z9" s="1">
+        <v>1.183906E-16</v>
+      </c>
+      <c r="AA9" s="1">
+        <v>3.4410190000000001E-4</v>
+      </c>
+      <c r="AB9" s="1">
+        <v>-4.5700780000000001E-16</v>
+      </c>
+      <c r="AC9" s="1">
+        <v>1.145764E-4</v>
+      </c>
+      <c r="AD9" s="1">
+        <v>2.0289420000000001E-5</v>
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11" s="1">
-        <v>-5.1623789999999997E-16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B12" s="1">
-        <v>4.14472E-6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>69</v>
-      </c>
-      <c r="B13" s="1">
-        <v>4.7219689999999997E-5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>70</v>
-      </c>
-      <c r="B14" s="1">
-        <v>2.229151E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B15" s="1">
-        <v>8.075933E-5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="28" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I28" t="s">
         <v>72</v>
-      </c>
-      <c r="B16" s="1">
-        <v>2.514372E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>73</v>
-      </c>
-      <c r="B17" s="1">
-        <v>5.9465829999999997E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B18" s="1">
-        <v>0.13074949999999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B19" s="1">
-        <v>0.30248510000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B20" s="1">
-        <v>5.3018290000000001E-4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B21" s="1">
-        <v>0.31595200000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B22" s="1">
-        <v>5.8977300000000003E-4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B23" s="1">
-        <v>8.5590240000000001E-3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B24" s="1">
-        <v>2.4154990000000001E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B25" s="1">
-        <v>1.0789860000000001E-3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B26" s="1">
-        <v>1.8113730000000001E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="B27" s="1">
-        <v>1.2349550000000001E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B28" s="1">
-        <v>2.6331760000000001E-3</v>
-      </c>
-      <c r="I28" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B29" s="1">
-        <v>2.6721660000000001E-4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="B30" s="1">
-        <v>4.3963509999999997E-3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B31" s="1">
-        <v>2.7584290000000001E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="B32" s="1">
-        <v>7.4017670000000001E-3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="B33" s="1">
-        <v>1.2460710000000001E-3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="B34" s="1">
-        <v>6.2941469999999999E-3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="B35" s="1">
-        <v>3.074902E-3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B36" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B37" s="1">
-        <v>2.1983469999999998E-3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="B38" s="1">
-        <v>3.6187070000000002E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>